<commit_message>
Modification dans la documentation
Ajout de certains points dans le journal de veille et également une petite modification dans le journal d'expérimentation
</commit_message>
<xml_diff>
--- a/Doc/JournalDeVeille.xlsx
+++ b/Doc/JournalDeVeille.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\1School1\Informatique\ProjetDApprofondissement2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\Unity\Approfondissement2\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5164DD-09EE-4B4A-9663-734B456E4692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826A01BE-49D6-4852-9074-38A5BA078234}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Journal de veille technologique</t>
   </si>
@@ -100,6 +100,19 @@
   </si>
   <si>
     <t>Le tutoriel permet la compréhension du contrôle de la camera lorsque le jeu est en cour d'exécusion.</t>
+  </si>
+  <si>
+    <t>Mixamo</t>
+  </si>
+  <si>
+    <t>1 févier 2021</t>
+  </si>
+  <si>
+    <t>Sur cette page web, plusieurs modèle étaient présent ainsi qu'une multitude d'animation, ces animations permettre d'être appliquer aux personnages dans unity.</t>
+  </si>
+  <si>
+    <t>Animation des personnages ainsi que modele
+https://www.mixamo.com/</t>
   </si>
 </sst>
 </file>
@@ -276,7 +289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -576,7 +589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -585,13 +598,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FC5144-D522-4A27-B795-CAA4CF26E9AA}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
@@ -628,7 +641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -776,12 +789,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout au journal d'experimentation
Ajout des problèmes rencontrés au journal d'expérimentation
</commit_message>
<xml_diff>
--- a/Doc/JournalDeVeille.xlsx
+++ b/Doc/JournalDeVeille.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\Unity\Approfondissement2\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\1School1\Informatique\ProjetDApprofondissement2\unityProject\unity\Approfondissement2\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826A01BE-49D6-4852-9074-38A5BA078234}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EE33EB-83BF-441C-ADCC-5A14F4657322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Journal de veille technologique</t>
   </si>
@@ -67,9 +67,6 @@
     <t>25 Janvier 2021</t>
   </si>
   <si>
-    <t>L'article présente les contrôles de base pour être en mesure de faire déplacer le personnage de base.</t>
-  </si>
-  <si>
     <t>Youtube</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>Tutoriel des bases de Unity https://www.youtube.com/watch?v=_QajrabyTJc</t>
-  </si>
-  <si>
-    <t>Le tutoriel permet de comprendre comment faire les mouvements de bases d'un personnage.</t>
   </si>
   <si>
     <t>Physique
@@ -92,16 +86,10 @@
     <t>26 janvier 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Le tutoriel permet de comprendre comment intégrer de la physique aux objects et aux personnages dans mon jeu. </t>
-  </si>
-  <si>
     <t>Control de la camera
 https://learn.unity.com/tutorial/controlling-unity-camera-behaviour</t>
   </si>
   <si>
-    <t>Le tutoriel permet la compréhension du contrôle de la camera lorsque le jeu est en cour d'exécusion.</t>
-  </si>
-  <si>
     <t>Mixamo</t>
   </si>
   <si>
@@ -113,13 +101,61 @@
   <si>
     <t>Animation des personnages ainsi que modele
 https://www.mixamo.com/</t>
+  </si>
+  <si>
+    <t>Importation d'un personnage et d'animation
+https://youtu.be/-FhvQDqmgmU?list=PL4PClcNOzNAuhVjD6HBRaIFedVndKsdwO</t>
+  </si>
+  <si>
+    <t>Annimation des personnages
+https://youtu.be/vApG8aYD5aI?list=PL4PClcNOzNAuhVjD6HBRaIFedVndKsdwO</t>
+  </si>
+  <si>
+    <t>1 février 2021</t>
+  </si>
+  <si>
+    <t>Dans le liens si joint, il est question du téléchargement, de l'importation et de la configuration des personnages. Dans la vidéo, nous pouvons voir la page web : "Mixamo", cette page permet de ce prrocurer plusieurs personnages différent, ainsi que plusieurs annimations gratuitement. Pour ce qui concerne l'importation et la configuration de ces personnages, nous devons simplement les glissers dans nos dossiers de projet et également modifier la configuration du matériel pour que celui-ci soit en "legacy".</t>
+  </si>
+  <si>
+    <t>Le tutoriel permet de comprendre comment faire les mouvements de bases d'un personnage. Il faut d'abord ajouter au personnage principal un "character controller" et par la suite, nous devons programmé ces mouvements de façon à ce que lorsque la souris est déplacée, la vision du personnage suive le mouvement de la souris ou encore lorsque nous appuyons sur les touches "w, a, s, d, espace" le personnage réagit d'une certaine façon.</t>
+  </si>
+  <si>
+    <t>L'article présente les contrôles de base pour être en mesure de faire déplacer le personnage de base. Ainsi que comment intégrer ces mouvements à nos personnages.</t>
+  </si>
+  <si>
+    <t>Le tutoriel permet de comprendre comment intégrer de la physique aux objets et aux personnages dans mon jeu. De plus, il nous présente comment appliquer cette physique à nos personnages de façon à rendre l'esthétique du jeu d'autant plus réaliste.</t>
+  </si>
+  <si>
+    <t>Le tutoriel permet la compréhension du contrôle de la caméra lorsque le jeu est en cour d'exécution. De plus, ce tutoriel présente comment utiliser la caméra telle la vision du personnage et également comment la déplace celle-ci pour rendre la chose encore plus réaliste.</t>
+  </si>
+  <si>
+    <t>Sur ce lien, il est question de comment intégrer les animations aux personnages et comment ceux-ci peuvent être activé. Tous d'abord, pour ajouter les animations aux personnages, nous devons créer un "animator controller" et par la suite l'appliquer au.x personnage.s en question. Par la suite, nous devons soit créer l'animation de toute pièce ou encore dans, si vous avez opter pour l'option Mixamo, vous pouvez également appliquer l'animation que vous avez téléchargée au préalable. Par la suite, vous allez devoir utiliser des scripts de façon à modifier l'animation des personnages selon les actions de ceux-ci.</t>
+  </si>
+  <si>
+    <t>Bibliographie</t>
+  </si>
+  <si>
+    <t>Nom du site</t>
+  </si>
+  <si>
+    <t>Liens</t>
+  </si>
+  <si>
+    <t>Utilité</t>
+  </si>
+  <si>
+    <t>Création de menu principale
+https://youtu.be/zc8ac_qUXQY?list=PL4PClcNOzNAuhVjD6HBRaIFedVndKsdwO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ce lien présente une façon de créer un menu principale, qui permet aux joueurs de soit commencer le jeu ou encore de le quitter si ceux-ci le désire. Dans la vidéo, nous pouvons voir comment </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +166,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -163,21 +205,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -289,7 +401,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -589,7 +701,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -598,13 +710,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FC5144-D522-4A27-B795-CAA4CF26E9AA}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
@@ -615,209 +727,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="E20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A18:E18"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Problème de collision avec des murs
Le problème qui était présent dans les version différente des npcs qui percutaient les murs sont parciellement régler.
</commit_message>
<xml_diff>
--- a/Doc/JournalDeVeille.xlsx
+++ b/Doc/JournalDeVeille.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\1School1\Informatique\ProjetDApprofondissement2\unityProject\unity\Approfondissement2\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\Unity\Approfondissement2\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EE33EB-83BF-441C-ADCC-5A14F4657322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34CA47E-AAAF-4842-AEDF-ABCB690AB864}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Journal de veille technologique</t>
   </si>
@@ -149,6 +149,63 @@
   </si>
   <si>
     <t xml:space="preserve">Ce lien présente une façon de créer un menu principale, qui permet aux joueurs de soit commencer le jeu ou encore de le quitter si ceux-ci le désire. Dans la vidéo, nous pouvons voir comment </t>
+  </si>
+  <si>
+    <t>2 février 2021</t>
+  </si>
+  <si>
+    <t>5 février 2021</t>
+  </si>
+  <si>
+    <t>Transition entre animation
+https://www.youtube.com/watch?v=FF6kezDQZ7s</t>
+  </si>
+  <si>
+    <t>Cette vidéo présente une manière de changer l'animation du personnage selon la touche qui est enfoncer. "Input.GetKey()" À l'aide de cette line, nous sommes en mesure d'activer des animations, mais pour ce faire, nous devons les avoirs programmer dans l'"Animator" avec des transitions entre ceux-ci.</t>
+  </si>
+  <si>
+    <t>Animation
+https://docs.unity3d.com/ScriptReference/Animation.Play.html</t>
+  </si>
+  <si>
+    <t>Ce lien présente une façon de créer un menu principale, qui permet d'animer le personnage. Tel que if(anim.isPlaying) et également anim.Play();</t>
+  </si>
+  <si>
+    <t>Capsule Collider
+https://docs.unity3d.com/ScriptReference/CapsuleCollider.html</t>
+  </si>
+  <si>
+    <t>Cette page présente la manière d'utiliser les capsules colliders fonctionnent, et les fonctionnalités de celle-ci. C'est-à-dire la collision entre d'autre collider.</t>
+  </si>
+  <si>
+    <t>GameObject
+https://docs.unity3d.com/ScriptReference/GameObject.html</t>
+  </si>
+  <si>
+    <t>Cette page présente qu'est-ce qu'un gameobject, ainsi que les utiliters de ceux-ci dans unity.</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Matériel</t>
+  </si>
+  <si>
+    <t>Cette page présente la façon sommaire de comment utiliser les matériaux dans Unity, ainsi que l'utiliter de ceux-ci. En bref, la page nous informes que les matériaux sont la manière principale de modifier le visuelle du jeux rapidement, ainsi que comment appliquer des textures à ces matériaux.</t>
+  </si>
+  <si>
+    <t>Terrain
+https://docs.unity3d.com/ScriptReference/Terrain.html</t>
+  </si>
+  <si>
+    <t>Cette page présente le fonctionnement du terrain dans Unity, ainsi que les modification qui peuvent être apporter à celui-ci. De plus, dans cette page vous pouvez voir différent outil utile à la modification du terrain.</t>
+  </si>
+  <si>
+    <t>RayCast
+https://www.youtube.com/watch?v=THnivyG0Mvo</t>
+  </si>
+  <si>
+    <t>Cette vidéo présente une face d'envoyer un rayon devant soit, pour détecter la collision avec d'autres objets. Si la collision a lieu, nous pouvons voir les informations de cette collision. Dans mon cas je voulais regarder le layer à laquelle la collision appartenait. Donc, puisque mon "layer" désirait portait le numéro 8, je vérifie que si la collision entre avec un objet de niveau 8 une action ce produit.</t>
   </si>
 </sst>
 </file>
@@ -197,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -209,21 +266,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -251,27 +293,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,17 +363,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,7 +500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -701,7 +800,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -712,330 +811,436 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FC5144-D522-4A27-B795-CAA4CF26E9AA}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="73" customWidth="1"/>
-    <col min="5" max="5" width="85.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="6" max="6" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:6" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="D11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="D12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="D15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="11" t="s">
+      <c r="D20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>3</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>4</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout d'un menu principal, ainsi qu'un menu de pause
</commit_message>
<xml_diff>
--- a/Doc/JournalDeVeille.xlsx
+++ b/Doc/JournalDeVeille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\Unity\Approfondissement2\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34CA47E-AAAF-4842-AEDF-ABCB690AB864}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171EE630-0B13-4EF9-8768-287C6FE462E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>Journal de veille technologique</t>
   </si>
@@ -188,9 +188,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>Matériel</t>
-  </si>
-  <si>
     <t>Cette page présente la façon sommaire de comment utiliser les matériaux dans Unity, ainsi que l'utiliter de ceux-ci. En bref, la page nous informes que les matériaux sont la manière principale de modifier le visuelle du jeux rapidement, ainsi que comment appliquer des textures à ces matériaux.</t>
   </si>
   <si>
@@ -206,6 +203,23 @@
   </si>
   <si>
     <t>Cette vidéo présente une face d'envoyer un rayon devant soit, pour détecter la collision avec d'autres objets. Si la collision a lieu, nous pouvons voir les informations de cette collision. Dans mon cas je voulais regarder le layer à laquelle la collision appartenait. Donc, puisque mon "layer" désirait portait le numéro 8, je vérifie que si la collision entre avec un objet de niveau 8 une action ce produit.</t>
+  </si>
+  <si>
+    <t>Matériel
+https://docs.unity3d.com/ScriptReference/Material.html</t>
+  </si>
+  <si>
+    <t>8 février 2021</t>
+  </si>
+  <si>
+    <t>9 février 2021</t>
+  </si>
+  <si>
+    <t>Menu Pause
+https://www.youtube.com/watch?v=JivuXdrIHK0</t>
+  </si>
+  <si>
+    <t>Cette vidéo permet de comprendre les bases de la création d'un menu pause, ainsi que les utilisations de celui-ci. C'est-à-dire le retour au menu principale, et même quitter le jeux.</t>
   </si>
 </sst>
 </file>
@@ -354,6 +368,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -362,33 +403,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,7 +826,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,14 +840,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -856,386 +870,392 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="9" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
-        <v>14</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>2</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>3</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>1</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>2</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>3</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="4">
         <v>4</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>